<commit_message>
20190522 tuan dui jiao yi
</commit_message>
<xml_diff>
--- a/体重记录.xlsx
+++ b/体重记录.xlsx
@@ -500,7 +500,7 @@
   <dimension ref="A1:G28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H12" sqref="H12"/>
+      <selection activeCell="F16" sqref="F16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -674,6 +674,12 @@
         <v>87</v>
       </c>
       <c r="D13" s="9"/>
+      <c r="F13" s="1">
+        <v>43606</v>
+      </c>
+      <c r="G13">
+        <v>89.8</v>
+      </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A14">

</xml_diff>